<commit_message>
added second trial with grayscale toggle
</commit_message>
<xml_diff>
--- a/queryImages.xlsx
+++ b/queryImages.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcogiven/PsychoPy/mock_study/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcogiven/Desktop/PsychoPyProjects/mock_study_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21F9F3A-BAAB-834C-86AB-FEAC95B774D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4549C77F-0E6E-A147-989F-2EC5949E2FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="26">
   <si>
     <t>query_image</t>
   </si>
@@ -116,6 +116,36 @@
   </si>
   <si>
     <t>image5</t>
+  </si>
+  <si>
+    <t>gray1</t>
+  </si>
+  <si>
+    <t>gray2</t>
+  </si>
+  <si>
+    <t>gray3</t>
+  </si>
+  <si>
+    <t>gray4</t>
+  </si>
+  <si>
+    <t>gray5</t>
+  </si>
+  <si>
+    <t>images/kiwi_gray.png</t>
+  </si>
+  <si>
+    <t>images/orange_gray.png</t>
+  </si>
+  <si>
+    <t>images/grape_gray.png</t>
+  </si>
+  <si>
+    <t>images/banana_gray.png</t>
+  </si>
+  <si>
+    <t>images/apple_gray.png</t>
   </si>
 </sst>
 </file>
@@ -507,11 +537,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -519,7 +549,7 @@
     <col min="1" max="1" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -541,8 +571,23 @@
       <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -564,8 +609,23 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -587,8 +647,23 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -610,8 +685,23 @@
       <c r="G4" t="s">
         <v>13</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -633,8 +723,23 @@
       <c r="G5" t="s">
         <v>13</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -655,6 +760,21 @@
       </c>
       <c r="G6" t="s">
         <v>15</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -670,21 +790,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F5CAB0486A994CA2C3B13E059EF2AE" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8645ec4a60d0c8c7009d2d6675847a91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="636d7205651659ec4fcda0bcbde9384b">
     <xsd:element name="properties">
@@ -798,10 +903,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF1C174-6AC6-4774-A736-3226A12360E4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -822,17 +950,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF1C174-6AC6-4774-A736-3226A12360E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>